<commit_message>
GenTopten2: echo hostname in messages
</commit_message>
<xml_diff>
--- a/SeasonData/Season-2017/SourceData-2017/PACTop10LCM-2017.xlsx
+++ b/SeasonData/Season-2017/SourceData-2017/PACTop10LCM-2017.xlsx
@@ -27779,22 +27779,22 @@
         <v>46.25</v>
       </c>
       <c r="G518" t="s">
-        <v>626</v>
+        <v>720</v>
       </c>
       <c r="H518" s="1" t="s">
-        <v>616</v>
+        <v>624</v>
       </c>
       <c r="I518" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="J518" t="s">
-        <v>627</v>
+        <v>721</v>
       </c>
       <c r="K518" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="L518" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
     </row>
     <row r="519" spans="1:12">
@@ -27817,22 +27817,22 @@
         <v>46.25</v>
       </c>
       <c r="G519" t="s">
-        <v>720</v>
+        <v>626</v>
       </c>
       <c r="H519" s="1" t="s">
-        <v>624</v>
+        <v>616</v>
       </c>
       <c r="I519" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="J519" t="s">
-        <v>721</v>
+        <v>627</v>
       </c>
       <c r="K519" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="L519" t="s">
-        <v>45</v>
+        <v>20</v>
       </c>
     </row>
     <row r="520" spans="1:12">
@@ -78502,9 +78502,11 @@
       <c r="J1857" t="s">
         <v>2246</v>
       </c>
-      <c r="K1857"/>
+      <c r="K1857" t="s">
+        <v>33</v>
+      </c>
       <c r="L1857" t="s">
-        <v>94</v>
+        <v>20</v>
       </c>
     </row>
     <row r="1858" spans="1:12">

</xml_diff>

<commit_message>
Misc changes to support our Linux port.
</commit_message>
<xml_diff>
--- a/SeasonData/Season-2017/SourceData-2017/PACTop10LCM-2017.xlsx
+++ b/SeasonData/Season-2017/SourceData-2017/PACTop10LCM-2017.xlsx
@@ -6869,16 +6869,16 @@
     <t>1:17.84</t>
   </si>
   <si>
+    <t xml:space="preserve"> Jim Kauffman</t>
+  </si>
+  <si>
+    <t>387Y-03JDZ</t>
+  </si>
+  <si>
     <t xml:space="preserve"> Christian P Hellwig</t>
   </si>
   <si>
     <t>387E-061HT</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Jim Kauffman</t>
-  </si>
-  <si>
-    <t>387Y-03JDZ</t>
   </si>
   <si>
     <t>1:20.67</t>
@@ -75418,10 +75418,10 @@
         <v>2284</v>
       </c>
       <c r="H1776" s="1" t="s">
-        <v>2243</v>
+        <v>2248</v>
       </c>
       <c r="I1776" s="1" t="s">
-        <v>358</v>
+        <v>219</v>
       </c>
       <c r="J1776" t="s">
         <v>2285</v>
@@ -75430,7 +75430,7 @@
         <v>33</v>
       </c>
       <c r="L1776" t="s">
-        <v>403</v>
+        <v>20</v>
       </c>
     </row>
     <row r="1777" spans="1:12">
@@ -75456,10 +75456,10 @@
         <v>2286</v>
       </c>
       <c r="H1777" s="1" t="s">
-        <v>2248</v>
+        <v>2243</v>
       </c>
       <c r="I1777" s="1" t="s">
-        <v>219</v>
+        <v>358</v>
       </c>
       <c r="J1777" t="s">
         <v>2287</v>
@@ -75468,7 +75468,7 @@
         <v>33</v>
       </c>
       <c r="L1777" t="s">
-        <v>20</v>
+        <v>403</v>
       </c>
     </row>
     <row r="1778" spans="1:12">
@@ -76213,7 +76213,7 @@
         <v>2320</v>
       </c>
       <c r="G1797" t="s">
-        <v>2284</v>
+        <v>2286</v>
       </c>
       <c r="H1797" s="1" t="s">
         <v>2243</v>
@@ -76222,7 +76222,7 @@
         <v>358</v>
       </c>
       <c r="J1797" t="s">
-        <v>2285</v>
+        <v>2287</v>
       </c>
       <c r="K1797" t="s">
         <v>2321</v>
@@ -76441,7 +76441,7 @@
         <v>2328</v>
       </c>
       <c r="G1803" t="s">
-        <v>2284</v>
+        <v>2286</v>
       </c>
       <c r="H1803" s="1" t="s">
         <v>2243</v>
@@ -76450,7 +76450,7 @@
         <v>358</v>
       </c>
       <c r="J1803" t="s">
-        <v>2285</v>
+        <v>2287</v>
       </c>
       <c r="K1803" t="s">
         <v>33</v>
@@ -76973,7 +76973,7 @@
         <v>44.46</v>
       </c>
       <c r="G1817" t="s">
-        <v>2284</v>
+        <v>2286</v>
       </c>
       <c r="H1817" s="1" t="s">
         <v>2243</v>
@@ -76982,7 +76982,7 @@
         <v>358</v>
       </c>
       <c r="J1817" t="s">
-        <v>2285</v>
+        <v>2287</v>
       </c>
       <c r="K1817" t="s">
         <v>2348</v>
@@ -77201,7 +77201,7 @@
         <v>2351</v>
       </c>
       <c r="G1823" t="s">
-        <v>2286</v>
+        <v>2284</v>
       </c>
       <c r="H1823" s="1" t="s">
         <v>2248</v>
@@ -77210,7 +77210,7 @@
         <v>219</v>
       </c>
       <c r="J1823" t="s">
-        <v>2287</v>
+        <v>2285</v>
       </c>
       <c r="K1823" t="s">
         <v>33</v>
@@ -77239,7 +77239,7 @@
         <v>2352</v>
       </c>
       <c r="G1824" t="s">
-        <v>2284</v>
+        <v>2286</v>
       </c>
       <c r="H1824" s="1" t="s">
         <v>2243</v>
@@ -77248,7 +77248,7 @@
         <v>358</v>
       </c>
       <c r="J1824" t="s">
-        <v>2285</v>
+        <v>2287</v>
       </c>
       <c r="K1824" t="s">
         <v>2348</v>
@@ -77467,7 +77467,7 @@
         <v>2358</v>
       </c>
       <c r="G1830" t="s">
-        <v>2284</v>
+        <v>2286</v>
       </c>
       <c r="H1830" s="1" t="s">
         <v>2243</v>
@@ -77476,7 +77476,7 @@
         <v>358</v>
       </c>
       <c r="J1830" t="s">
-        <v>2285</v>
+        <v>2287</v>
       </c>
       <c r="K1830" t="s">
         <v>2321</v>
@@ -78502,11 +78502,9 @@
       <c r="J1857" t="s">
         <v>2246</v>
       </c>
-      <c r="K1857" t="s">
-        <v>33</v>
-      </c>
+      <c r="K1857"/>
       <c r="L1857" t="s">
-        <v>20</v>
+        <v>94</v>
       </c>
     </row>
     <row r="1858" spans="1:12">
@@ -78605,7 +78603,7 @@
         <v>38.04</v>
       </c>
       <c r="G1860" t="s">
-        <v>2286</v>
+        <v>2284</v>
       </c>
       <c r="H1860" s="1" t="s">
         <v>2248</v>
@@ -78614,7 +78612,7 @@
         <v>219</v>
       </c>
       <c r="J1860" t="s">
-        <v>2287</v>
+        <v>2285</v>
       </c>
       <c r="K1860" t="s">
         <v>33</v>
@@ -78681,7 +78679,7 @@
         <v>47.38</v>
       </c>
       <c r="G1862" t="s">
-        <v>2284</v>
+        <v>2286</v>
       </c>
       <c r="H1862" s="1" t="s">
         <v>2243</v>
@@ -78690,7 +78688,7 @@
         <v>358</v>
       </c>
       <c r="J1862" t="s">
-        <v>2285</v>
+        <v>2287</v>
       </c>
       <c r="K1862" t="s">
         <v>2348</v>
@@ -79437,7 +79435,7 @@
         <v>2396</v>
       </c>
       <c r="G1882" t="s">
-        <v>2284</v>
+        <v>2286</v>
       </c>
       <c r="H1882" s="1" t="s">
         <v>2243</v>
@@ -79446,7 +79444,7 @@
         <v>358</v>
       </c>
       <c r="J1882" t="s">
-        <v>2285</v>
+        <v>2287</v>
       </c>
       <c r="K1882" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
fixed DoFetchAndProcessTopten to print out a bit more useful info; fixed Topten2.pl to get the fake races data from a different place, and moved those files.
</commit_message>
<xml_diff>
--- a/SeasonData/Season-2017/SourceData-2017/PACTop10LCM-2017.xlsx
+++ b/SeasonData/Season-2017/SourceData-2017/PACTop10LCM-2017.xlsx
@@ -6869,16 +6869,16 @@
     <t>1:17.84</t>
   </si>
   <si>
+    <t xml:space="preserve"> Christian P Hellwig</t>
+  </si>
+  <si>
+    <t>387E-061HT</t>
+  </si>
+  <si>
     <t xml:space="preserve"> Jim Kauffman</t>
   </si>
   <si>
     <t>387Y-03JDZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Christian P Hellwig</t>
-  </si>
-  <si>
-    <t>387E-061HT</t>
   </si>
   <si>
     <t>1:20.67</t>
@@ -75418,10 +75418,10 @@
         <v>2284</v>
       </c>
       <c r="H1776" s="1" t="s">
-        <v>2248</v>
+        <v>2243</v>
       </c>
       <c r="I1776" s="1" t="s">
-        <v>219</v>
+        <v>358</v>
       </c>
       <c r="J1776" t="s">
         <v>2285</v>
@@ -75430,7 +75430,7 @@
         <v>33</v>
       </c>
       <c r="L1776" t="s">
-        <v>20</v>
+        <v>403</v>
       </c>
     </row>
     <row r="1777" spans="1:12">
@@ -75456,10 +75456,10 @@
         <v>2286</v>
       </c>
       <c r="H1777" s="1" t="s">
-        <v>2243</v>
+        <v>2248</v>
       </c>
       <c r="I1777" s="1" t="s">
-        <v>358</v>
+        <v>219</v>
       </c>
       <c r="J1777" t="s">
         <v>2287</v>
@@ -75468,7 +75468,7 @@
         <v>33</v>
       </c>
       <c r="L1777" t="s">
-        <v>403</v>
+        <v>20</v>
       </c>
     </row>
     <row r="1778" spans="1:12">
@@ -76213,7 +76213,7 @@
         <v>2320</v>
       </c>
       <c r="G1797" t="s">
-        <v>2286</v>
+        <v>2284</v>
       </c>
       <c r="H1797" s="1" t="s">
         <v>2243</v>
@@ -76222,7 +76222,7 @@
         <v>358</v>
       </c>
       <c r="J1797" t="s">
-        <v>2287</v>
+        <v>2285</v>
       </c>
       <c r="K1797" t="s">
         <v>2321</v>
@@ -76441,7 +76441,7 @@
         <v>2328</v>
       </c>
       <c r="G1803" t="s">
-        <v>2286</v>
+        <v>2284</v>
       </c>
       <c r="H1803" s="1" t="s">
         <v>2243</v>
@@ -76450,7 +76450,7 @@
         <v>358</v>
       </c>
       <c r="J1803" t="s">
-        <v>2287</v>
+        <v>2285</v>
       </c>
       <c r="K1803" t="s">
         <v>33</v>
@@ -76973,7 +76973,7 @@
         <v>44.46</v>
       </c>
       <c r="G1817" t="s">
-        <v>2286</v>
+        <v>2284</v>
       </c>
       <c r="H1817" s="1" t="s">
         <v>2243</v>
@@ -76982,7 +76982,7 @@
         <v>358</v>
       </c>
       <c r="J1817" t="s">
-        <v>2287</v>
+        <v>2285</v>
       </c>
       <c r="K1817" t="s">
         <v>2348</v>
@@ -77201,7 +77201,7 @@
         <v>2351</v>
       </c>
       <c r="G1823" t="s">
-        <v>2284</v>
+        <v>2286</v>
       </c>
       <c r="H1823" s="1" t="s">
         <v>2248</v>
@@ -77210,7 +77210,7 @@
         <v>219</v>
       </c>
       <c r="J1823" t="s">
-        <v>2285</v>
+        <v>2287</v>
       </c>
       <c r="K1823" t="s">
         <v>33</v>
@@ -77239,7 +77239,7 @@
         <v>2352</v>
       </c>
       <c r="G1824" t="s">
-        <v>2286</v>
+        <v>2284</v>
       </c>
       <c r="H1824" s="1" t="s">
         <v>2243</v>
@@ -77248,7 +77248,7 @@
         <v>358</v>
       </c>
       <c r="J1824" t="s">
-        <v>2287</v>
+        <v>2285</v>
       </c>
       <c r="K1824" t="s">
         <v>2348</v>
@@ -77467,7 +77467,7 @@
         <v>2358</v>
       </c>
       <c r="G1830" t="s">
-        <v>2286</v>
+        <v>2284</v>
       </c>
       <c r="H1830" s="1" t="s">
         <v>2243</v>
@@ -77476,7 +77476,7 @@
         <v>358</v>
       </c>
       <c r="J1830" t="s">
-        <v>2287</v>
+        <v>2285</v>
       </c>
       <c r="K1830" t="s">
         <v>2321</v>
@@ -78603,7 +78603,7 @@
         <v>38.04</v>
       </c>
       <c r="G1860" t="s">
-        <v>2284</v>
+        <v>2286</v>
       </c>
       <c r="H1860" s="1" t="s">
         <v>2248</v>
@@ -78612,7 +78612,7 @@
         <v>219</v>
       </c>
       <c r="J1860" t="s">
-        <v>2285</v>
+        <v>2287</v>
       </c>
       <c r="K1860" t="s">
         <v>33</v>
@@ -78679,7 +78679,7 @@
         <v>47.38</v>
       </c>
       <c r="G1862" t="s">
-        <v>2286</v>
+        <v>2284</v>
       </c>
       <c r="H1862" s="1" t="s">
         <v>2243</v>
@@ -78688,7 +78688,7 @@
         <v>358</v>
       </c>
       <c r="J1862" t="s">
-        <v>2287</v>
+        <v>2285</v>
       </c>
       <c r="K1862" t="s">
         <v>2348</v>
@@ -79435,7 +79435,7 @@
         <v>2396</v>
       </c>
       <c r="G1882" t="s">
-        <v>2286</v>
+        <v>2284</v>
       </c>
       <c r="H1882" s="1" t="s">
         <v>2243</v>
@@ -79444,7 +79444,7 @@
         <v>358</v>
       </c>
       <c r="J1882" t="s">
-        <v>2287</v>
+        <v>2285</v>
       </c>
       <c r="K1882" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
Updated script to supply hostname in subject and message.
</commit_message>
<xml_diff>
--- a/SeasonData/Season-2017/SourceData-2017/PACTop10LCM-2017.xlsx
+++ b/SeasonData/Season-2017/SourceData-2017/PACTop10LCM-2017.xlsx
@@ -27779,22 +27779,22 @@
         <v>46.25</v>
       </c>
       <c r="G518" t="s">
-        <v>720</v>
+        <v>626</v>
       </c>
       <c r="H518" s="1" t="s">
-        <v>624</v>
+        <v>616</v>
       </c>
       <c r="I518" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="J518" t="s">
-        <v>721</v>
+        <v>627</v>
       </c>
       <c r="K518" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="L518" t="s">
-        <v>45</v>
+        <v>20</v>
       </c>
     </row>
     <row r="519" spans="1:12">
@@ -27817,22 +27817,22 @@
         <v>46.25</v>
       </c>
       <c r="G519" t="s">
-        <v>626</v>
+        <v>720</v>
       </c>
       <c r="H519" s="1" t="s">
-        <v>616</v>
+        <v>624</v>
       </c>
       <c r="I519" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="J519" t="s">
-        <v>627</v>
+        <v>721</v>
       </c>
       <c r="K519" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="L519" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
     </row>
     <row r="520" spans="1:12">
@@ -78502,9 +78502,11 @@
       <c r="J1857" t="s">
         <v>2246</v>
       </c>
-      <c r="K1857"/>
+      <c r="K1857" t="s">
+        <v>33</v>
+      </c>
       <c r="L1857" t="s">
-        <v>94</v>
+        <v>20</v>
       </c>
     </row>
     <row r="1858" spans="1:12">

</xml_diff>